<commit_message>
Record Dashboard sanity button reult in Excel
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/DashboardButton.xlsx
+++ b/Aml_automation/src/Common/DashboardButton.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
   <si>
     <t>PostTilte</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Future brand club collaborator role isha</t>
+  </si>
+  <si>
+    <t>Future brand club coordinator role isha</t>
+  </si>
+  <si>
+    <t>shobha</t>
+  </si>
+  <si>
+    <t>Future brand longform coordinator role isha</t>
+  </si>
+  <si>
+    <t>Future slideshow post editor role isha</t>
+  </si>
+  <si>
+    <t>coordinator post longform :- Sumit</t>
+  </si>
+  <si>
+    <t>coordinatorIsha</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>director</t>
   </si>
 </sst>
 </file>
@@ -506,6 +533,238 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sanity testing files for all Editorial roles
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/DashboardButton.xlsx
+++ b/Aml_automation/src/Common/DashboardButton.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="30">
   <si>
     <t>PostTilte</t>
   </si>
@@ -765,6 +765,35 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Excel File- Dashboard Button
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/DashboardButton.xlsx
+++ b/Aml_automation/src/Common/DashboardButton.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agile\Automation\Aml_automation\src\Common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AML-2\git\Automation\Aml_automation\src\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23475" windowHeight="7005" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DashboardButton" sheetId="1" r:id="rId1"/>
     <sheet name="TODOSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="republishFilter" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>PostTilte</t>
   </si>
@@ -62,6 +63,27 @@
   </si>
   <si>
     <t>Buttons</t>
+  </si>
+  <si>
+    <t>PostTitle</t>
+  </si>
+  <si>
+    <t>Logged_In_Author</t>
+  </si>
+  <si>
+    <t>AuthorName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title_matching </t>
+  </si>
+  <si>
+    <t>Post_content_match</t>
+  </si>
+  <si>
+    <t>Title_keyword_match</t>
+  </si>
+  <si>
+    <t>Post_Keyword_match</t>
   </si>
 </sst>
 </file>
@@ -117,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -131,6 +153,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -526,4 +550,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="48" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel file for republicado search
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/DashboardButton.xlsx
+++ b/Aml_automation/src/Common/DashboardButton.xlsx
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -101,6 +101,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -153,8 +160,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +501,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD13"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +564,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,5 +618,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lfe post type check added
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/DashboardButton.xlsx
+++ b/Aml_automation/src/Common/DashboardButton.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AML-2\git\Automation\Aml_automation\src\Common\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="53">
   <si>
     <t>PostTilte</t>
   </si>
@@ -84,13 +84,110 @@
   </si>
   <si>
     <t>Post_Keyword_match</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/preview-main/216902/49ac542f5119512682b72f1d44e6fe81</t>
+  </si>
+  <si>
+    <t>nobodyuser</t>
+  </si>
+  <si>
+    <t>schedule</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>Repost,Editar,Pasar a borrador,Destacar</t>
+  </si>
+  <si>
+    <t>Repost,Pasar a borrador,Editar,Destacar</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/analisis/tt</t>
+  </si>
+  <si>
+    <t>Repost,Rechazar,Editar,Destacar</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/cazando-gangas/shobha-testing-new-post-fro-instagram-feeds</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/aplicaciones/test-cf-post-123</t>
+  </si>
+  <si>
+    <t>club</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/basics/test-cf-post-basics</t>
+  </si>
+  <si>
+    <t>Repost,Editar,Quitar de portad</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/citroenelectricos/isha-brand-cf</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/analisis/slideshow-post-isha</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/entrevistas/normal-video-post-2-pankaj</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/n/isha-brand-article</t>
+  </si>
+  <si>
+    <t>isha_bcol</t>
+  </si>
+  <si>
+    <t>Club</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/entrevistas/normal-video-post-1-pankaj</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/especiales/shobha-testing-future-post-entendiendo-que-mayores-revoluciones-industria-desarrollo-78687</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/analisis/hola-hola-test</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/citroenelectricos/isha-brand-cf-post</t>
+  </si>
+  <si>
+    <t>isha_bcor</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/componentes/testing-date-issue</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/componentes/testing-normal-post-publish</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/n/que-le-preguntarias-a-astronoma</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/componentes/testing-title</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/audio/isha-cms-post</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -450,15 +547,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="57" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="57.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -488,6 +585,528 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -506,16 +1125,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -569,16 +1188,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" customWidth="1"/>
-    <col min="8" max="8" width="48" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>